<commit_message>
added tests to layout spreadsheet
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\eclipse-workspace\ClueProject\ClueProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\eclipse-workspace\ClueProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BABA52-B8D3-4016-AB25-3B9D8F5CC174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AD89C8-6E6A-49A3-A9DE-54190C404EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64EDCF6C-983A-4D65-9789-1C28D60B590E}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,11 +1469,11 @@
       <c r="R12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S12" s="5" t="s">
+      <c r="S12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T12" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>1</v>
       </c>
       <c r="U12" s="4" t="s">
         <v>1</v>
@@ -2319,11 +2319,11 @@
       <c r="H23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>1</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>29</v>

</xml_diff>